<commit_message>
menyelsaikan pengecekan dan perlu penambahan parameter pengecekan
</commit_message>
<xml_diff>
--- a/NOV 2024 2024_MSLSINVDIST.xlsx
+++ b/NOV 2024 2024_MSLSINVDIST.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cek\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT-Aplikasi SPV\Documents\ASIATOP\Cek\CekSID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC212F06-3804-4323-9EFC-E2BF533C4AF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC89430A-AEAD-47F2-870E-8B729963B8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25020" yWindow="1305" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -1394,30 +1394,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7A3EDEE-945D-4631-9436-C34F0AA2C526}">
   <dimension ref="A1:O413"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A388" workbookViewId="0">
-      <selection activeCell="E403" sqref="E403"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>32</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>32</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>32</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>32</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>19</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>21</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>21</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>22</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>22</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>23</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>23</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>24</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>25</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>25</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>25</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>26</v>
       </c>
@@ -2787,7 +2787,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>26</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>26</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>26</v>
       </c>
@@ -2934,7 +2934,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>26</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>26</v>
       </c>
@@ -3032,7 +3032,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>26</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>27</v>
       </c>
@@ -3130,7 +3130,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>28</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>29</v>
       </c>
@@ -3228,7 +3228,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>29</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>30</v>
       </c>
@@ -3326,7 +3326,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>31</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>33</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>33</v>
       </c>
@@ -3473,7 +3473,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>33</v>
       </c>
@@ -3522,7 +3522,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>33</v>
       </c>
@@ -3571,7 +3571,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>33</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>34</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>35</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>35</v>
       </c>
@@ -3767,7 +3767,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>36</v>
       </c>
@@ -3816,7 +3816,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>36</v>
       </c>
@@ -3865,7 +3865,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>36</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>37</v>
       </c>
@@ -3963,7 +3963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>37</v>
       </c>
@@ -4012,7 +4012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>37</v>
       </c>
@@ -4061,7 +4061,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>37</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>37</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>37</v>
       </c>
@@ -4208,7 +4208,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>38</v>
       </c>
@@ -4257,7 +4257,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>38</v>
       </c>
@@ -4306,7 +4306,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>39</v>
       </c>
@@ -4355,7 +4355,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>39</v>
       </c>
@@ -4404,7 +4404,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>40</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>40</v>
       </c>
@@ -4502,7 +4502,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>40</v>
       </c>
@@ -4551,7 +4551,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>40</v>
       </c>
@@ -4600,7 +4600,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>41</v>
       </c>
@@ -4649,7 +4649,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>41</v>
       </c>
@@ -4698,7 +4698,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>41</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>41</v>
       </c>
@@ -4796,7 +4796,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>41</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>41</v>
       </c>
@@ -4894,7 +4894,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>42</v>
       </c>
@@ -4943,7 +4943,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>42</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>42</v>
       </c>
@@ -5041,7 +5041,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>42</v>
       </c>
@@ -5090,7 +5090,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>42</v>
       </c>
@@ -5139,7 +5139,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>43</v>
       </c>
@@ -5188,7 +5188,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>43</v>
       </c>
@@ -5237,7 +5237,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>44</v>
       </c>
@@ -5286,7 +5286,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>44</v>
       </c>
@@ -5335,7 +5335,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>44</v>
       </c>
@@ -5384,7 +5384,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>45</v>
       </c>
@@ -5433,7 +5433,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>45</v>
       </c>
@@ -5482,7 +5482,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>45</v>
       </c>
@@ -5531,7 +5531,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>45</v>
       </c>
@@ -5580,7 +5580,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>46</v>
       </c>
@@ -5629,7 +5629,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>47</v>
       </c>
@@ -5678,7 +5678,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>48</v>
       </c>
@@ -5727,7 +5727,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>48</v>
       </c>
@@ -5776,7 +5776,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>48</v>
       </c>
@@ -5825,7 +5825,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>48</v>
       </c>
@@ -5874,7 +5874,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>48</v>
       </c>
@@ -5923,7 +5923,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>48</v>
       </c>
@@ -5972,7 +5972,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>49</v>
       </c>
@@ -6021,7 +6021,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>49</v>
       </c>
@@ -6070,7 +6070,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>49</v>
       </c>
@@ -6119,7 +6119,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>49</v>
       </c>
@@ -6168,7 +6168,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>49</v>
       </c>
@@ -6217,7 +6217,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>49</v>
       </c>
@@ -6266,7 +6266,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>49</v>
       </c>
@@ -6315,7 +6315,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>50</v>
       </c>
@@ -6364,7 +6364,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>50</v>
       </c>
@@ -6413,7 +6413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>50</v>
       </c>
@@ -6462,7 +6462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>50</v>
       </c>
@@ -6511,7 +6511,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>51</v>
       </c>
@@ -6560,7 +6560,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>51</v>
       </c>
@@ -6609,7 +6609,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>52</v>
       </c>
@@ -6658,7 +6658,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>53</v>
       </c>
@@ -6707,7 +6707,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>53</v>
       </c>
@@ -6756,7 +6756,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>54</v>
       </c>
@@ -6805,7 +6805,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>55</v>
       </c>
@@ -6854,7 +6854,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>55</v>
       </c>
@@ -6903,7 +6903,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>55</v>
       </c>
@@ -6952,7 +6952,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>55</v>
       </c>
@@ -7001,7 +7001,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>55</v>
       </c>
@@ -7050,7 +7050,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>56</v>
       </c>
@@ -7099,7 +7099,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>56</v>
       </c>
@@ -7148,7 +7148,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>56</v>
       </c>
@@ -7197,7 +7197,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>56</v>
       </c>
@@ -7246,7 +7246,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>56</v>
       </c>
@@ -7295,7 +7295,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>56</v>
       </c>
@@ -7344,7 +7344,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>56</v>
       </c>
@@ -7393,7 +7393,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>57</v>
       </c>
@@ -7442,7 +7442,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>57</v>
       </c>
@@ -7491,7 +7491,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
         <v>57</v>
       </c>
@@ -7540,7 +7540,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>57</v>
       </c>
@@ -7589,7 +7589,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>57</v>
       </c>
@@ -7638,7 +7638,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>57</v>
       </c>
@@ -7687,7 +7687,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
         <v>58</v>
       </c>
@@ -7736,7 +7736,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>58</v>
       </c>
@@ -7785,7 +7785,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
         <v>58</v>
       </c>
@@ -7834,7 +7834,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
         <v>58</v>
       </c>
@@ -7883,7 +7883,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
         <v>59</v>
       </c>
@@ -7932,7 +7932,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
         <v>59</v>
       </c>
@@ -7981,7 +7981,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
         <v>59</v>
       </c>
@@ -8030,7 +8030,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
         <v>60</v>
       </c>
@@ -8079,7 +8079,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
         <v>61</v>
       </c>
@@ -8128,7 +8128,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
         <v>61</v>
       </c>
@@ -8177,7 +8177,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
         <v>62</v>
       </c>
@@ -8226,7 +8226,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
         <v>62</v>
       </c>
@@ -8275,7 +8275,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
         <v>62</v>
       </c>
@@ -8324,7 +8324,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
         <v>63</v>
       </c>
@@ -8373,7 +8373,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
         <v>64</v>
       </c>
@@ -8422,7 +8422,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
         <v>65</v>
       </c>
@@ -8471,7 +8471,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
         <v>65</v>
       </c>
@@ -8520,7 +8520,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
         <v>65</v>
       </c>
@@ -8569,7 +8569,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
         <v>65</v>
       </c>
@@ -8618,7 +8618,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
         <v>65</v>
       </c>
@@ -8667,7 +8667,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
         <v>66</v>
       </c>
@@ -8716,7 +8716,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
         <v>66</v>
       </c>
@@ -8765,7 +8765,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
         <v>67</v>
       </c>
@@ -8814,7 +8814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
         <v>67</v>
       </c>
@@ -8863,7 +8863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
         <v>67</v>
       </c>
@@ -8912,7 +8912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
         <v>67</v>
       </c>
@@ -8961,7 +8961,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
         <v>68</v>
       </c>
@@ -9010,7 +9010,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
         <v>69</v>
       </c>
@@ -9059,7 +9059,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
         <v>69</v>
       </c>
@@ -9108,7 +9108,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
         <v>69</v>
       </c>
@@ -9157,7 +9157,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
         <v>69</v>
       </c>
@@ -9206,7 +9206,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
         <v>70</v>
       </c>
@@ -9255,7 +9255,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
         <v>70</v>
       </c>
@@ -9304,7 +9304,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
         <v>70</v>
       </c>
@@ -9353,7 +9353,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A163" s="4" t="s">
         <v>70</v>
       </c>
@@ -9402,7 +9402,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
         <v>70</v>
       </c>
@@ -9451,7 +9451,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
         <v>70</v>
       </c>
@@ -9500,7 +9500,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A166" s="4" t="s">
         <v>71</v>
       </c>
@@ -9549,7 +9549,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
         <v>71</v>
       </c>
@@ -9598,7 +9598,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
         <v>71</v>
       </c>
@@ -9647,7 +9647,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A169" s="14" t="s">
         <v>72</v>
       </c>
@@ -9696,7 +9696,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A170" s="14" t="s">
         <v>72</v>
       </c>
@@ -9745,7 +9745,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
         <v>73</v>
       </c>
@@ -9794,7 +9794,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
         <v>73</v>
       </c>
@@ -9843,7 +9843,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A173" s="4" t="s">
         <v>74</v>
       </c>
@@ -9892,7 +9892,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
         <v>74</v>
       </c>
@@ -9941,7 +9941,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A175" s="4" t="s">
         <v>74</v>
       </c>
@@ -9990,7 +9990,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
         <v>74</v>
       </c>
@@ -10039,7 +10039,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A177" s="4" t="s">
         <v>74</v>
       </c>
@@ -10088,7 +10088,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A178" s="4" t="s">
         <v>75</v>
       </c>
@@ -10137,7 +10137,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A179" s="4" t="s">
         <v>76</v>
       </c>
@@ -10186,7 +10186,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A180" s="4" t="s">
         <v>76</v>
       </c>
@@ -10235,7 +10235,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A181" s="4" t="s">
         <v>77</v>
       </c>
@@ -10284,7 +10284,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A182" s="4" t="s">
         <v>77</v>
       </c>
@@ -10333,7 +10333,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A183" s="4" t="s">
         <v>77</v>
       </c>
@@ -10382,7 +10382,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A184" s="4" t="s">
         <v>77</v>
       </c>
@@ -10431,7 +10431,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A185" s="4" t="s">
         <v>77</v>
       </c>
@@ -10480,7 +10480,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A186" s="4" t="s">
         <v>77</v>
       </c>
@@ -10529,7 +10529,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A187" s="4" t="s">
         <v>78</v>
       </c>
@@ -10578,7 +10578,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A188" s="4" t="s">
         <v>78</v>
       </c>
@@ -10627,7 +10627,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A189" s="4" t="s">
         <v>78</v>
       </c>
@@ -10676,7 +10676,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A190" s="4" t="s">
         <v>78</v>
       </c>
@@ -10725,7 +10725,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A191" s="4" t="s">
         <v>78</v>
       </c>
@@ -10774,7 +10774,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A192" s="4" t="s">
         <v>78</v>
       </c>
@@ -10823,7 +10823,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A193" s="4" t="s">
         <v>79</v>
       </c>
@@ -10872,7 +10872,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A194" s="4" t="s">
         <v>79</v>
       </c>
@@ -10921,7 +10921,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A195" s="4" t="s">
         <v>80</v>
       </c>
@@ -10970,7 +10970,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A196" s="4" t="s">
         <v>81</v>
       </c>
@@ -11019,7 +11019,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A197" s="4" t="s">
         <v>81</v>
       </c>
@@ -11068,7 +11068,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A198" s="4" t="s">
         <v>82</v>
       </c>
@@ -11117,7 +11117,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A199" s="4" t="s">
         <v>83</v>
       </c>
@@ -11166,7 +11166,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A200" s="4" t="s">
         <v>83</v>
       </c>
@@ -11215,7 +11215,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A201" s="4" t="s">
         <v>83</v>
       </c>
@@ -11264,7 +11264,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="202" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A202" s="4" t="s">
         <v>83</v>
       </c>
@@ -11313,7 +11313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A203" s="4" t="s">
         <v>83</v>
       </c>
@@ -11362,7 +11362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="204" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A204" s="4" t="s">
         <v>84</v>
       </c>
@@ -11411,7 +11411,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="205" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A205" s="4" t="s">
         <v>85</v>
       </c>
@@ -11460,7 +11460,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="206" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A206" s="4" t="s">
         <v>86</v>
       </c>
@@ -11509,7 +11509,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A207" s="4" t="s">
         <v>86</v>
       </c>
@@ -11558,7 +11558,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A208" s="4" t="s">
         <v>86</v>
       </c>
@@ -11607,7 +11607,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="209" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A209" s="4" t="s">
         <v>86</v>
       </c>
@@ -11656,7 +11656,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="210" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A210" s="4" t="s">
         <v>87</v>
       </c>
@@ -11705,7 +11705,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="211" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A211" s="4" t="s">
         <v>87</v>
       </c>
@@ -11754,7 +11754,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="212" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A212" s="4" t="s">
         <v>88</v>
       </c>
@@ -11803,7 +11803,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="213" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A213" s="4" t="s">
         <v>88</v>
       </c>
@@ -11852,7 +11852,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="214" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A214" s="4" t="s">
         <v>88</v>
       </c>
@@ -11901,7 +11901,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="215" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A215" s="4" t="s">
         <v>89</v>
       </c>
@@ -11950,7 +11950,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="216" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A216" s="4" t="s">
         <v>90</v>
       </c>
@@ -11999,7 +11999,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="217" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A217" s="4" t="s">
         <v>90</v>
       </c>
@@ -12048,7 +12048,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="218" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A218" s="4" t="s">
         <v>90</v>
       </c>
@@ -12097,7 +12097,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="219" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A219" s="4" t="s">
         <v>90</v>
       </c>
@@ -12146,7 +12146,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="220" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A220" s="4" t="s">
         <v>90</v>
       </c>
@@ -12195,7 +12195,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="221" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A221" s="4" t="s">
         <v>90</v>
       </c>
@@ -12244,7 +12244,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="222" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A222" s="4" t="s">
         <v>90</v>
       </c>
@@ -12293,7 +12293,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="223" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A223" s="4" t="s">
         <v>91</v>
       </c>
@@ -12342,7 +12342,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="224" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A224" s="4" t="s">
         <v>91</v>
       </c>
@@ -12391,7 +12391,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="225" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A225" s="4" t="s">
         <v>91</v>
       </c>
@@ -12440,7 +12440,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="226" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A226" s="4" t="s">
         <v>91</v>
       </c>
@@ -12489,7 +12489,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="227" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A227" s="4" t="s">
         <v>92</v>
       </c>
@@ -12538,7 +12538,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="228" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A228" s="4" t="s">
         <v>93</v>
       </c>
@@ -12587,7 +12587,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="229" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A229" s="4" t="s">
         <v>93</v>
       </c>
@@ -12636,7 +12636,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="230" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A230" s="4" t="s">
         <v>94</v>
       </c>
@@ -12685,7 +12685,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="231" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A231" s="4" t="s">
         <v>94</v>
       </c>
@@ -12734,7 +12734,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="232" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A232" s="4" t="s">
         <v>95</v>
       </c>
@@ -12783,7 +12783,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="233" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A233" s="4" t="s">
         <v>95</v>
       </c>
@@ -12832,7 +12832,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="234" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A234" s="4" t="s">
         <v>95</v>
       </c>
@@ -12881,7 +12881,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="235" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A235" s="4" t="s">
         <v>96</v>
       </c>
@@ -12930,7 +12930,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="236" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A236" s="4" t="s">
         <v>96</v>
       </c>
@@ -12979,7 +12979,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="237" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A237" s="4" t="s">
         <v>96</v>
       </c>
@@ -13028,7 +13028,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="238" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A238" s="4" t="s">
         <v>96</v>
       </c>
@@ -13077,7 +13077,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="239" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A239" s="4" t="s">
         <v>96</v>
       </c>
@@ -13126,7 +13126,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="240" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A240" s="4" t="s">
         <v>96</v>
       </c>
@@ -13175,7 +13175,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="241" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A241" s="4" t="s">
         <v>97</v>
       </c>
@@ -13224,7 +13224,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="242" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A242" s="4" t="s">
         <v>98</v>
       </c>
@@ -13273,7 +13273,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="243" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A243" s="4" t="s">
         <v>99</v>
       </c>
@@ -13322,7 +13322,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="244" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A244" s="4" t="s">
         <v>100</v>
       </c>
@@ -13371,7 +13371,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="245" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A245" s="4" t="s">
         <v>101</v>
       </c>
@@ -13420,7 +13420,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="246" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A246" s="4" t="s">
         <v>101</v>
       </c>
@@ -13469,7 +13469,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="247" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A247" s="4" t="s">
         <v>101</v>
       </c>
@@ -13518,7 +13518,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="248" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A248" s="4" t="s">
         <v>102</v>
       </c>
@@ -13567,7 +13567,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="249" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A249" s="4" t="s">
         <v>102</v>
       </c>
@@ -13616,7 +13616,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="250" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A250" s="4" t="s">
         <v>102</v>
       </c>
@@ -13665,7 +13665,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="251" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A251" s="4" t="s">
         <v>102</v>
       </c>
@@ -13714,7 +13714,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="252" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A252" s="4" t="s">
         <v>103</v>
       </c>
@@ -13763,7 +13763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="253" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A253" s="4" t="s">
         <v>103</v>
       </c>
@@ -13812,7 +13812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="254" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A254" s="4" t="s">
         <v>103</v>
       </c>
@@ -13861,7 +13861,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="255" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A255" s="4" t="s">
         <v>104</v>
       </c>
@@ -13910,7 +13910,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="256" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A256" s="4" t="s">
         <v>104</v>
       </c>
@@ -13959,7 +13959,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="257" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A257" s="4" t="s">
         <v>104</v>
       </c>
@@ -14008,7 +14008,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="258" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A258" s="4" t="s">
         <v>104</v>
       </c>
@@ -14057,7 +14057,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="259" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A259" s="4" t="s">
         <v>104</v>
       </c>
@@ -14106,7 +14106,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="260" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A260" s="4" t="s">
         <v>104</v>
       </c>
@@ -14155,7 +14155,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="261" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A261" s="4" t="s">
         <v>104</v>
       </c>
@@ -14204,7 +14204,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="262" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A262" s="4" t="s">
         <v>104</v>
       </c>
@@ -14253,7 +14253,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="263" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A263" s="4" t="s">
         <v>105</v>
       </c>
@@ -14302,7 +14302,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="264" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A264" s="4" t="s">
         <v>106</v>
       </c>
@@ -14351,7 +14351,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="265" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A265" s="4" t="s">
         <v>106</v>
       </c>
@@ -14400,7 +14400,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="266" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A266" s="4" t="s">
         <v>106</v>
       </c>
@@ -14449,7 +14449,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="267" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A267" s="4" t="s">
         <v>107</v>
       </c>
@@ -14498,7 +14498,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="268" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A268" s="4" t="s">
         <v>107</v>
       </c>
@@ -14547,7 +14547,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="269" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A269" s="4" t="s">
         <v>108</v>
       </c>
@@ -14596,7 +14596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="270" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A270" s="4" t="s">
         <v>108</v>
       </c>
@@ -14645,7 +14645,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="271" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A271" s="4" t="s">
         <v>108</v>
       </c>
@@ -14694,7 +14694,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="272" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A272" s="4" t="s">
         <v>108</v>
       </c>
@@ -14743,7 +14743,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="273" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A273" s="4" t="s">
         <v>108</v>
       </c>
@@ -14792,7 +14792,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="274" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A274" s="4" t="s">
         <v>108</v>
       </c>
@@ -14841,7 +14841,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="275" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A275" s="4" t="s">
         <v>108</v>
       </c>
@@ -14890,7 +14890,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="276" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A276" s="4" t="s">
         <v>108</v>
       </c>
@@ -14939,7 +14939,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="277" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A277" s="4" t="s">
         <v>109</v>
       </c>
@@ -14988,7 +14988,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="278" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A278" s="4" t="s">
         <v>110</v>
       </c>
@@ -15037,7 +15037,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="279" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A279" s="4" t="s">
         <v>110</v>
       </c>
@@ -15086,7 +15086,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="280" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A280" s="4" t="s">
         <v>110</v>
       </c>
@@ -15135,7 +15135,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="281" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A281" s="4" t="s">
         <v>110</v>
       </c>
@@ -15184,7 +15184,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="282" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A282" s="4" t="s">
         <v>110</v>
       </c>
@@ -15233,7 +15233,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="283" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A283" s="4" t="s">
         <v>110</v>
       </c>
@@ -15282,7 +15282,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="284" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A284" s="4" t="s">
         <v>111</v>
       </c>
@@ -15331,7 +15331,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="285" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A285" s="4" t="s">
         <v>112</v>
       </c>
@@ -15380,7 +15380,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="286" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A286" s="4" t="s">
         <v>112</v>
       </c>
@@ -15429,7 +15429,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="287" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A287" s="4" t="s">
         <v>112</v>
       </c>
@@ -15478,7 +15478,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="288" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A288" s="4" t="s">
         <v>112</v>
       </c>
@@ -15527,7 +15527,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="289" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A289" s="4" t="s">
         <v>113</v>
       </c>
@@ -15576,7 +15576,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="290" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A290" s="4" t="s">
         <v>113</v>
       </c>
@@ -15625,7 +15625,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="291" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A291" s="4" t="s">
         <v>113</v>
       </c>
@@ -15674,7 +15674,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="292" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A292" s="4" t="s">
         <v>113</v>
       </c>
@@ -15723,7 +15723,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="293" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A293" s="4" t="s">
         <v>114</v>
       </c>
@@ -15772,7 +15772,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="294" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A294" s="4" t="s">
         <v>114</v>
       </c>
@@ -15821,7 +15821,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="295" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A295" s="4" t="s">
         <v>115</v>
       </c>
@@ -15870,7 +15870,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="296" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A296" s="4" t="s">
         <v>115</v>
       </c>
@@ -15919,7 +15919,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="297" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A297" s="4" t="s">
         <v>115</v>
       </c>
@@ -15968,7 +15968,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="298" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A298" s="4" t="s">
         <v>115</v>
       </c>
@@ -16017,7 +16017,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="299" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A299" s="4" t="s">
         <v>116</v>
       </c>
@@ -16066,7 +16066,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="300" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A300" s="4" t="s">
         <v>116</v>
       </c>
@@ -16115,7 +16115,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="301" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A301" s="4" t="s">
         <v>117</v>
       </c>
@@ -16164,7 +16164,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="302" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A302" s="4" t="s">
         <v>117</v>
       </c>
@@ -16213,7 +16213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="303" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A303" s="4" t="s">
         <v>118</v>
       </c>
@@ -16262,7 +16262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="304" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A304" s="4" t="s">
         <v>119</v>
       </c>
@@ -16311,7 +16311,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="305" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A305" s="4" t="s">
         <v>119</v>
       </c>
@@ -16360,7 +16360,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="306" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A306" s="4" t="s">
         <v>119</v>
       </c>
@@ -16409,7 +16409,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="307" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A307" s="4" t="s">
         <v>119</v>
       </c>
@@ -16458,7 +16458,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="308" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A308" s="4" t="s">
         <v>119</v>
       </c>
@@ -16507,7 +16507,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="309" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A309" s="4" t="s">
         <v>119</v>
       </c>
@@ -16556,7 +16556,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="310" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A310" s="4" t="s">
         <v>120</v>
       </c>
@@ -16605,7 +16605,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="311" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A311" s="4" t="s">
         <v>120</v>
       </c>
@@ -16654,7 +16654,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="312" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A312" s="4" t="s">
         <v>120</v>
       </c>
@@ -16703,7 +16703,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="313" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A313" s="4" t="s">
         <v>120</v>
       </c>
@@ -16752,7 +16752,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="314" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A314" s="4" t="s">
         <v>121</v>
       </c>
@@ -16801,7 +16801,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="315" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A315" s="4" t="s">
         <v>121</v>
       </c>
@@ -16850,7 +16850,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="316" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A316" s="4" t="s">
         <v>121</v>
       </c>
@@ -16899,7 +16899,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="317" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A317" s="4" t="s">
         <v>121</v>
       </c>
@@ -16948,7 +16948,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="318" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A318" s="4" t="s">
         <v>121</v>
       </c>
@@ -16997,7 +16997,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="319" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A319" s="4" t="s">
         <v>122</v>
       </c>
@@ -17046,7 +17046,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="320" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A320" s="4" t="s">
         <v>123</v>
       </c>
@@ -17095,7 +17095,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="321" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A321" s="4" t="s">
         <v>123</v>
       </c>
@@ -17144,7 +17144,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="322" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A322" s="4" t="s">
         <v>123</v>
       </c>
@@ -17193,7 +17193,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="323" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A323" s="4" t="s">
         <v>124</v>
       </c>
@@ -17242,7 +17242,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="324" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A324" s="4" t="s">
         <v>124</v>
       </c>
@@ -17291,7 +17291,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="325" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A325" s="4" t="s">
         <v>124</v>
       </c>
@@ -17340,7 +17340,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="326" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A326" s="4" t="s">
         <v>125</v>
       </c>
@@ -17389,7 +17389,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="327" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A327" s="4" t="s">
         <v>126</v>
       </c>
@@ -17438,7 +17438,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="328" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A328" s="4" t="s">
         <v>127</v>
       </c>
@@ -17487,7 +17487,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="329" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A329" s="4" t="s">
         <v>127</v>
       </c>
@@ -17536,7 +17536,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="330" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A330" s="4" t="s">
         <v>127</v>
       </c>
@@ -17585,7 +17585,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="331" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A331" s="4" t="s">
         <v>127</v>
       </c>
@@ -17634,7 +17634,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="332" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A332" s="4" t="s">
         <v>128</v>
       </c>
@@ -17683,7 +17683,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="333" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A333" s="4" t="s">
         <v>128</v>
       </c>
@@ -17732,7 +17732,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="334" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A334" s="4" t="s">
         <v>129</v>
       </c>
@@ -17781,7 +17781,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="335" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A335" s="4" t="s">
         <v>130</v>
       </c>
@@ -17830,7 +17830,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="336" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A336" s="4" t="s">
         <v>131</v>
       </c>
@@ -17879,7 +17879,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="337" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A337" s="4" t="s">
         <v>131</v>
       </c>
@@ -17928,7 +17928,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="338" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A338" s="4" t="s">
         <v>132</v>
       </c>
@@ -17977,7 +17977,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="339" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A339" s="4" t="s">
         <v>133</v>
       </c>
@@ -18026,7 +18026,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="340" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A340" s="4" t="s">
         <v>133</v>
       </c>
@@ -18075,7 +18075,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="341" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A341" s="4" t="s">
         <v>133</v>
       </c>
@@ -18124,7 +18124,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="342" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A342" s="4" t="s">
         <v>133</v>
       </c>
@@ -18173,7 +18173,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="343" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A343" s="4" t="s">
         <v>133</v>
       </c>
@@ -18222,7 +18222,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="344" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A344" s="4" t="s">
         <v>134</v>
       </c>
@@ -18271,7 +18271,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="345" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A345" s="4" t="s">
         <v>134</v>
       </c>
@@ -18320,7 +18320,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="346" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A346" s="4" t="s">
         <v>134</v>
       </c>
@@ -18369,7 +18369,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="347" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A347" s="4" t="s">
         <v>134</v>
       </c>
@@ -18418,7 +18418,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="348" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A348" s="4" t="s">
         <v>135</v>
       </c>
@@ -18467,7 +18467,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="349" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A349" s="4" t="s">
         <v>135</v>
       </c>
@@ -18516,7 +18516,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="350" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A350" s="4" t="s">
         <v>135</v>
       </c>
@@ -18565,7 +18565,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="351" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A351" s="4" t="s">
         <v>136</v>
       </c>
@@ -18614,7 +18614,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="352" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A352" s="4" t="s">
         <v>136</v>
       </c>
@@ -18663,7 +18663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="353" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A353" s="4" t="s">
         <v>136</v>
       </c>
@@ -18712,7 +18712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="354" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A354" s="4" t="s">
         <v>136</v>
       </c>
@@ -18761,7 +18761,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="355" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A355" s="4" t="s">
         <v>136</v>
       </c>
@@ -18810,7 +18810,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="356" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A356" s="4" t="s">
         <v>137</v>
       </c>
@@ -18859,7 +18859,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="357" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A357" s="4" t="s">
         <v>137</v>
       </c>
@@ -18908,7 +18908,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="358" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A358" s="4" t="s">
         <v>137</v>
       </c>
@@ -18957,7 +18957,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="359" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A359" s="4" t="s">
         <v>138</v>
       </c>
@@ -19006,7 +19006,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="360" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A360" s="4" t="s">
         <v>138</v>
       </c>
@@ -19055,7 +19055,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="361" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A361" s="4" t="s">
         <v>138</v>
       </c>
@@ -19104,7 +19104,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="362" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A362" s="4" t="s">
         <v>139</v>
       </c>
@@ -19153,7 +19153,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="363" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A363" s="4" t="s">
         <v>139</v>
       </c>
@@ -19202,7 +19202,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="364" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A364" s="4" t="s">
         <v>139</v>
       </c>
@@ -19251,7 +19251,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="365" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A365" s="4" t="s">
         <v>139</v>
       </c>
@@ -19300,7 +19300,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="366" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A366" s="4" t="s">
         <v>139</v>
       </c>
@@ -19349,7 +19349,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="367" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A367" s="4" t="s">
         <v>139</v>
       </c>
@@ -19398,7 +19398,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="368" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A368" s="4" t="s">
         <v>140</v>
       </c>
@@ -19447,7 +19447,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="369" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A369" s="4" t="s">
         <v>140</v>
       </c>
@@ -19496,7 +19496,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="370" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A370" s="4" t="s">
         <v>140</v>
       </c>
@@ -19545,7 +19545,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="371" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A371" s="4" t="s">
         <v>140</v>
       </c>
@@ -19594,7 +19594,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="372" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A372" s="4" t="s">
         <v>141</v>
       </c>
@@ -19643,7 +19643,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="373" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A373" s="4" t="s">
         <v>141</v>
       </c>
@@ -19692,7 +19692,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="374" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A374" s="4" t="s">
         <v>141</v>
       </c>
@@ -19741,7 +19741,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="375" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A375" s="4" t="s">
         <v>141</v>
       </c>
@@ -19790,7 +19790,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="376" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A376" s="4" t="s">
         <v>142</v>
       </c>
@@ -19839,7 +19839,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="377" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A377" s="4" t="s">
         <v>142</v>
       </c>
@@ -19888,7 +19888,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="378" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A378" s="4" t="s">
         <v>142</v>
       </c>
@@ -19937,7 +19937,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="379" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A379" s="4" t="s">
         <v>143</v>
       </c>
@@ -19986,7 +19986,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="380" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A380" s="4" t="s">
         <v>144</v>
       </c>
@@ -20035,7 +20035,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="381" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A381" s="4" t="s">
         <v>144</v>
       </c>
@@ -20084,7 +20084,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="382" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A382" s="4" t="s">
         <v>145</v>
       </c>
@@ -20133,7 +20133,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="383" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A383" s="4" t="s">
         <v>145</v>
       </c>
@@ -20182,7 +20182,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="384" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A384" s="4" t="s">
         <v>145</v>
       </c>
@@ -20231,7 +20231,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="385" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A385" s="4" t="s">
         <v>145</v>
       </c>
@@ -20280,7 +20280,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="386" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A386" s="4" t="s">
         <v>146</v>
       </c>
@@ -20319,7 +20319,7 @@
         <v>37840</v>
       </c>
       <c r="M386" s="1">
-        <f t="shared" ref="M386:M449" si="13">L386*1.11</f>
+        <f t="shared" ref="M386:M413" si="13">L386*1.11</f>
         <v>42002.400000000001</v>
       </c>
       <c r="N386" t="s">
@@ -20329,7 +20329,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="387" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A387" s="4" t="s">
         <v>146</v>
       </c>
@@ -20378,7 +20378,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="388" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A388" s="4" t="s">
         <v>146</v>
       </c>
@@ -20427,7 +20427,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="389" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A389" s="4" t="s">
         <v>146</v>
       </c>
@@ -20476,7 +20476,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="390" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A390" s="4" t="s">
         <v>146</v>
       </c>
@@ -20525,7 +20525,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="391" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A391" s="4" t="s">
         <v>147</v>
       </c>
@@ -20574,7 +20574,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="392" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A392" s="4" t="s">
         <v>147</v>
       </c>
@@ -20623,7 +20623,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="393" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A393" s="4" t="s">
         <v>147</v>
       </c>
@@ -20672,7 +20672,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="394" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A394" s="4" t="s">
         <v>147</v>
       </c>
@@ -20721,7 +20721,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="395" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A395" s="4" t="s">
         <v>147</v>
       </c>
@@ -20770,7 +20770,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="396" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A396" s="4" t="s">
         <v>147</v>
       </c>
@@ -20819,7 +20819,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="397" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A397" s="4" t="s">
         <v>148</v>
       </c>
@@ -20868,7 +20868,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="398" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A398" s="4" t="s">
         <v>148</v>
       </c>
@@ -20917,7 +20917,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="399" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A399" s="4" t="s">
         <v>149</v>
       </c>
@@ -20966,7 +20966,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="400" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A400" s="4" t="s">
         <v>149</v>
       </c>
@@ -21015,7 +21015,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="401" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A401" s="4" t="s">
         <v>149</v>
       </c>
@@ -21064,7 +21064,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="402" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A402" s="4" t="s">
         <v>149</v>
       </c>
@@ -21113,7 +21113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="403" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A403" s="4" t="s">
         <v>149</v>
       </c>
@@ -21162,7 +21162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="404" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A404" s="4" t="s">
         <v>149</v>
       </c>
@@ -21211,7 +21211,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="405" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A405" s="4" t="s">
         <v>149</v>
       </c>
@@ -21260,7 +21260,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="406" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A406" s="4" t="s">
         <v>149</v>
       </c>
@@ -21309,7 +21309,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="407" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A407" s="4" t="s">
         <v>149</v>
       </c>
@@ -21358,7 +21358,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="408" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A408" s="4" t="s">
         <v>149</v>
       </c>
@@ -21407,7 +21407,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="409" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A409" s="4" t="s">
         <v>149</v>
       </c>
@@ -21456,7 +21456,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="410" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A410" s="4" t="s">
         <v>149</v>
       </c>
@@ -21505,7 +21505,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="411" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A411" s="4" t="s">
         <v>150</v>
       </c>
@@ -21554,7 +21554,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="412" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A412" s="4" t="s">
         <v>150</v>
       </c>
@@ -21603,7 +21603,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="413" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A413" s="20" t="s">
         <v>293</v>
       </c>

</xml_diff>